<commit_message>
Further CrewMember code tidy. Localization-based fixes and fix for CreateFile being used instead of CreateTeamMemberFile.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Editor/Localization/SUGARUnityLocalization.xlsx
+++ b/stm-unity/Assets/Editor/Localization/SUGARUnityLocalization.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="120">
   <si>
     <t>Key</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>Punteggio</t>
+  </si>
+  <si>
+    <t>GROUP_MEMBERS_LOAD_ERROR</t>
   </si>
 </sst>
 </file>
@@ -762,7 +765,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -927,8 +930,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
+      <c r="A15" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>82</v>

</xml_diff>